<commit_message>
Minor changes to the fuel calculation table
</commit_message>
<xml_diff>
--- a/Fuel calculations.xlsx
+++ b/Fuel calculations.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
   <si>
     <t>Engine displacement [m3]</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>Test mass</t>
+  </si>
+  <si>
+    <t>Pulse time per cylinder [100th ms]</t>
   </si>
 </sst>
 </file>
@@ -499,15 +502,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -788,11 +791,20 @@
         <v>4.4958924453689413</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20">
+        <f>B19*100</f>
+        <v>449.58924453689411</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
         <v>27</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <f>B14*B17/60000</f>
         <v>4.8503643413853879E-5</v>
       </c>

</xml_diff>